<commit_message>
add tests and test data for alttpr.scanner
</commit_message>
<xml_diff>
--- a/tests/data/stats_df_2024-06-15_REFERENCE.xlsx
+++ b/tests/data/stats_df_2024-06-15_REFERENCE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8b0bd3a772d8ada/Dokumente/Projekte/alttpr/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_339D57825BD05225B7B92C11595ED87656CD3211" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28AB8C02-393F-4959-A8D6-4EB341B4CECC}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_339D57825BD05225B7B92C11595ED87656CD3211" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03276D68-0BAD-45AB-9CA0-1FE29C59A0FE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Gewinnertyp - In 59 ALttPR Community-/Weekly-Races war Dennsen86 auf dem Treppchen! Das sind 27% von insgesamt 217 Races</t>
   </si>
   <si>
-    <t>10006</t>
-  </si>
-  <si>
-    <t>Berühmter Streamer kann's nicht lassen: Zuletzt stand Dennsen86 beim ALttPR Community-/Weekly-Race vor 6 Tagen auf dem Treppchen (2.Platz)</t>
-  </si>
-  <si>
     <t>10007</t>
   </si>
   <si>
@@ -179,18 +173,6 @@
   </si>
   <si>
     <t>Endlich frei - Für Open-Seeds benötigte Dennsen86 im Schnitt 01:40:21 ALttPR in 92 Races.</t>
-  </si>
-  <si>
-    <t>10031</t>
-  </si>
-  <si>
-    <t>Gut gemacht: Dennsen86 hat mit 01:22:55 beim letzten ALttPR Community-/Weekly-Race vor 6 Tagen den 2.Platz belegt.</t>
-  </si>
-  <si>
-    <t>10032</t>
-  </si>
-  <si>
-    <t>Volles Haus - 16 Racer waren beim ALttPR Community-/Weekly-Race vor 6 Tagen dabei.</t>
   </si>
   <si>
     <t>100000</t>
@@ -562,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,30 +766,6 @@
       </c>
       <c r="B27" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>